<commit_message>
Added search by floor functionality, Updated test sample excel sheet
</commit_message>
<xml_diff>
--- a/examples.xlsx
+++ b/examples.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22819"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_3144\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3E039C0-B3E9-45A1-BABF-ED0628BA0F85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B177759F-C3A5-46B0-8819-84BBEAF3C8E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$W$999</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$X$999</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,12 +38,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="54">
   <si>
-    <t>Unique code</t>
+    <t>Location</t>
   </si>
   <si>
     <t>Flat #</t>
+  </si>
+  <si>
+    <t>Floor</t>
   </si>
   <si>
     <t>Bedroom</t>
@@ -64,7 +67,7 @@
     <t>Balcony</t>
   </si>
   <si>
-    <t>Available from</t>
+    <t>Available</t>
   </si>
   <si>
     <t>Description</t>
@@ -149,6 +152,54 @@
   </si>
   <si>
     <t xml:space="preserve">Spacious 2 bed dual aspect flat which includes an in-built wardrobe and an en-suite in the master bedroom, a large utility storage cupboard, a modern bathroom with heated towel rack, integrated kitchen appliances and washing and dryer machine. The flat also benefits from a large private balcony </t>
+  </si>
+  <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>Spacious 2 bedroom 2 bathroom flat with a west facing balcony overlooking the private courtyard. Boasting an open plan kitchen and living area, en suite bathroom and in-built wardrobes in the master bedroom and storage room. The kicthen is fully integrated with Bosch appliances including fridge, freezer, electric hob, oven, microwave and dishwasher. There is also a washer and dryer machine in the utility room.</t>
+  </si>
+  <si>
+    <t>Spacious 1 bedroom dual aspect flat with large double bedroom which has in-built wardrobes The flat includes a large private balcony, modern bathroom, large utility room an open plan kitchen and living area. The kitchen is fully integrated with Bosch appliances including fridge, freezer, electric hob, oven, microwave, dishwasher and washer/dryer machine.</t>
+  </si>
+  <si>
+    <t>Dual aspect 1 bedroom flat boasting a double bedroom with built in wardrobes, modern bathroom, large utility room and an open plan kicthen and living area which is fully integrated with fridge, freezer, electric hob, microwave, dish washer and washer/dryer machine. The flat also benefits from a south facing balcony.</t>
+  </si>
+  <si>
+    <t>1 bedroom south facing flat with built in wardrobes, modern bathroom, large utility room and an open plan kicthen and living area which is fully integrated with fridge, freezer, electric hob, microwave, dish washer and washer/dryer machine.</t>
+  </si>
+  <si>
+    <t>Spacious 1 bedroom dual aspect west facing flat with large double bedroom which has in-built wardrobes The flat includes a large private balcony, modern bathroom, large utility room an open plan kitchen and living area. The kitchen is fully integrated with Bosch appliances including fridge, freezer, electric hob, oven, microwave, dishwasher and washer/dryer machine.</t>
+  </si>
+  <si>
+    <t>Spacious 2 bedroom 2 bathroom dual aspect west facing flats with in-built wardrobes and en-suite in the master bedroom. The flat benefits from a large private balcony, modern bathroom, large utility room an open plan kitchen and living area. The kitchen is fully integrated with Bosch appliances including fridge, freezer, electric hob, oven, microwave, dishwasher and washer/dryer machine.</t>
+  </si>
+  <si>
+    <t>Very spacious 2 bedroom dual aspect flat with a south facing private balcony, modern and stylish fully integarted kitchen, open plan living area, large storage room and a family bathroom. The master bedroom benefits from en-suite bathroom and in-built wardrobes.</t>
+  </si>
+  <si>
+    <t>Spacious 2 bedroom 2 bathroom dual aspect flats with in-built wardrobes and en-suite in the master bedroom. The flat benefits from a large private balcony, modern bathroom, large utility room an open plan kitchen and living area. The kitchen is fully integrated with Bosch appliances including fridge, freezer, electric hob, oven, microwave, dishwasher and washer/dryer machine.</t>
+  </si>
+  <si>
+    <t>Spacious 2 bedroom 2 bathroom dual aspect east facing flats with in-built wardrobes and en-suite in the master bedroom. The flat benefits from a large private balcony, modern bathroom, large utility room an open plan kitchen and living area. The kitchen is fully integrated with Bosch appliances including fridge, freezer, electric hob, oven, microwave, dishwasher and washer/dryer machine.</t>
+  </si>
+  <si>
+    <t>Spacious 2 bedroom 2 bathroom flat with a large private west facing balcony overlooking the private courtyard. Boasting an open plan kitchen and living area, en suite bathroom and in-built wardrobes in the master bedroom and storage room. The kicthen is fully integrated with Bosch appliances including fridge, freezer, electric hob, oven, microwave and dishwasher. There is also a washer and dryer machine in the utility room.</t>
+  </si>
+  <si>
+    <t>Stunning and spacious 3 bedroom flat with a large open plan kitchen and living area, two modern bathrooms, with the en-suite in the master bedroom and a utility room. The kitchen is fully integrated with Bosch appliances including fridge, freezer, electric hb, oven, microwave, dishwasher. There is also a washer and dryer in the utility room. The flat benefits from a west facing balcony large enough to play Cricket on!</t>
+  </si>
+  <si>
+    <t>Stunning and spacious 3 bedroom flat with a large open plan kitchen and living area, two modern bathrooms, with the en-suite in the master bedroom and a utility room. The kitchen is fully integrated with Bosch appliances including fridge, freezer, electric hb, oven, microwave, dishwasher. There is also a washer and dryer in the utility room. The flat benefits from a east facing balcony large enough to play Cricket on!</t>
+  </si>
+  <si>
+    <t>Spacious 2 bedroom 2 bathroom penthouse flat with a large east facing privcate balcony, en-suite and built in wardrobes in the master bedroom, open plan kitchen and living area, a fully integrated kitchen including fridge, freezer, electric hob, oven, microwave, dishwasner and washer and dryerlocated in the utility room.</t>
+  </si>
+  <si>
+    <t>Spacious 2 bedroom 2 bathroom penthouse flat with a large west facing privcate balcony, en-suite and built in wardrobes in the master bedroom, open plan kitchen and living area, a fully integrated kitchen including fridge, freezer, electric hob, oven, microwave, dishwasner and washer and dryerlocated in the utility room.</t>
+  </si>
+  <si>
+    <t>1 bedroom south facing penthouse flat with built in wardrobes, modern bathroom, large utility room and an open plan kicthen and living area which is fully integrated with fridge, freezer, electric hob, microwave, dish washer and washer/dryer machine.</t>
   </si>
 </sst>
 </file>
@@ -435,24 +486,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P999"/>
+  <dimension ref="A1:Q999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="14.625" customWidth="1"/>
-    <col min="4" max="8" width="8.5" customWidth="1"/>
-    <col min="9" max="9" width="10.375" customWidth="1"/>
-    <col min="10" max="10" width="65.125" customWidth="1"/>
-    <col min="11" max="23" width="8.5" customWidth="1"/>
+    <col min="2" max="3" width="9" customWidth="1"/>
+    <col min="4" max="4" width="14.625" customWidth="1"/>
+    <col min="5" max="9" width="8.5" customWidth="1"/>
+    <col min="10" max="10" width="10.375" customWidth="1"/>
+    <col min="11" max="11" width="65.125" customWidth="1"/>
+    <col min="12" max="24" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" customHeight="1">
+    <row r="1" spans="1:17" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -477,511 +528,2364 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="15.75" customHeight="1">
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="C2" s="3">
-        <v>1</v>
-      </c>
-      <c r="D2" s="10">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="10">
         <v>764</v>
       </c>
-      <c r="E2" s="10">
-        <v>2</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="11">
+      <c r="F2" s="10">
+        <v>2</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="11">
         <v>2130</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="3"/>
+      <c r="J2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="10">
+        <v>522</v>
+      </c>
+      <c r="F3" s="10">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="11">
+        <v>1560</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="5">
+        <v>44031</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1">
+        <v>928</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="3">
-        <v>2</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="10">
-        <v>522</v>
-      </c>
-      <c r="E3" s="10">
-        <v>1</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="11">
-        <v>1560</v>
-      </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="5">
-        <v>44031</v>
-      </c>
-      <c r="J3" s="4" t="s">
+      <c r="H4" s="1">
+        <v>2365</v>
+      </c>
+      <c r="J4" s="5">
+        <v>43960</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>509</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="1">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1">
-        <v>928</v>
-      </c>
-      <c r="E4" s="1">
-        <v>2</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="1">
-        <v>2365</v>
-      </c>
-      <c r="I4" s="5">
-        <v>43960</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1">
-        <v>509</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="1">
+      <c r="H5" s="1">
         <v>1500</v>
       </c>
-      <c r="H5" s="1">
-        <v>1</v>
-      </c>
-      <c r="I5" s="5">
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+      <c r="J5" s="5">
         <v>43992</v>
       </c>
-      <c r="J5" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="59.25" customHeight="1">
+      <c r="K5" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="59.25" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1">
         <v>67</v>
       </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
         <v>525</v>
       </c>
-      <c r="E6" s="1">
-        <v>1</v>
-      </c>
-      <c r="F6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="1">
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="1">
         <v>1200</v>
       </c>
-      <c r="H6" s="1">
-        <v>1</v>
-      </c>
-      <c r="I6" s="8">
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
+      <c r="J6" s="8">
         <v>44051</v>
       </c>
-      <c r="J6" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="K6" s="9"/>
+      <c r="K6" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
       <c r="O6" s="9"/>
       <c r="P6" s="9"/>
-    </row>
-    <row r="7" spans="1:16" ht="15.75" customHeight="1">
+      <c r="Q6" s="9"/>
+    </row>
+    <row r="7" spans="1:17" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1">
         <v>68</v>
       </c>
-      <c r="C7" s="1">
-        <v>2</v>
-      </c>
+      <c r="C7" s="1"/>
       <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1">
         <v>907</v>
       </c>
-      <c r="E7" s="1">
-        <v>2</v>
-      </c>
-      <c r="F7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="1">
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="1">
         <v>1500</v>
       </c>
-      <c r="H7" s="1">
-        <v>1</v>
-      </c>
-      <c r="I7" s="5">
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
+      <c r="J7" s="5">
         <v>44080</v>
       </c>
-      <c r="J7" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="15.75" customHeight="1">
+      <c r="K7" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1">
         <v>13</v>
       </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
+      <c r="C8" s="1"/>
       <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
         <v>622</v>
       </c>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="F8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="9">
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="9">
         <v>1415</v>
       </c>
-      <c r="I8" s="5">
+      <c r="J8" s="5">
         <v>43985</v>
       </c>
-      <c r="J8" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="15.75" customHeight="1">
+      <c r="K8" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1">
         <v>14</v>
       </c>
-      <c r="C9" s="1">
-        <v>1</v>
-      </c>
+      <c r="C9" s="1"/>
       <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
         <v>582</v>
       </c>
-      <c r="E9" s="1">
-        <v>1</v>
-      </c>
-      <c r="F9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="1">
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="1">
         <v>1575</v>
       </c>
-      <c r="H9" s="1">
-        <v>1</v>
-      </c>
-      <c r="I9" s="5">
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
+      <c r="J9" s="5">
         <v>44059</v>
       </c>
-      <c r="J9" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="15.75" customHeight="1">
+      <c r="K9" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1">
         <v>15</v>
       </c>
-      <c r="C10" s="1">
-        <v>2</v>
-      </c>
+      <c r="C10" s="1"/>
       <c r="D10" s="1">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1">
         <v>776</v>
       </c>
-      <c r="E10" s="1">
-        <v>2</v>
-      </c>
-      <c r="F10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="1">
+      <c r="F10" s="1">
+        <v>2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="1">
         <v>17</v>
       </c>
-      <c r="H10" s="1">
-        <v>1</v>
-      </c>
-      <c r="I10" s="5">
+      <c r="I10" s="1">
+        <v>1</v>
+      </c>
+      <c r="J10" s="5">
         <v>44016</v>
       </c>
-      <c r="J10" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="15.75" customHeight="1">
+      <c r="K10" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B11" s="1">
         <v>23</v>
       </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
+      <c r="C11" s="1"/>
       <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
         <v>599</v>
       </c>
-      <c r="E11" s="1">
-        <v>1</v>
-      </c>
-      <c r="F11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="1">
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="1">
         <v>1545</v>
       </c>
-      <c r="I11" s="5">
+      <c r="J11" s="5">
         <v>44034</v>
       </c>
-      <c r="J11" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="15.75" customHeight="1">
+      <c r="K11" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="15.75" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B12" s="1">
         <v>24</v>
       </c>
-      <c r="C12" s="1">
-        <v>2</v>
-      </c>
+      <c r="C12" s="1"/>
       <c r="D12" s="1">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1">
         <v>771</v>
       </c>
-      <c r="E12" s="1">
-        <v>2</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="F12" s="1">
+        <v>2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1785</v>
+      </c>
+      <c r="J12" s="5">
+        <v>43983</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>764</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="K13" s="7"/>
+      <c r="L13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>522</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="K14" s="7"/>
+      <c r="L14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>474</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="K15" s="9"/>
+      <c r="L15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>610</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="K16" s="9"/>
+      <c r="L16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>527</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="K17" s="9"/>
+      <c r="L17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>517</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="K18" s="7"/>
+      <c r="L18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19">
+        <v>7</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>527</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="K19" s="7"/>
+      <c r="L19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>576</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="K20" s="7"/>
+      <c r="L20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21">
+        <v>9</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>764</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="K21" s="7"/>
+      <c r="L21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22">
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>522</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="K22" s="7"/>
+      <c r="L22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23">
+        <v>11</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23">
+        <v>474</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="K23" s="9"/>
+      <c r="L23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24">
+        <v>12</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>630</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="K24" s="9"/>
+      <c r="L24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25">
+        <v>13</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>527</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="K25" s="9"/>
+      <c r="L25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26">
+        <v>14</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>517</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="K26" s="7"/>
+      <c r="L26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27">
         <v>15</v>
       </c>
-      <c r="G12" s="1">
-        <v>1785</v>
-      </c>
-      <c r="I12" s="5">
-        <v>43983</v>
-      </c>
-      <c r="J12" s="4" t="s">
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27">
+        <v>527</v>
+      </c>
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="K27" s="7"/>
+      <c r="L27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28">
+        <v>16</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28">
+        <v>667</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="K28" s="7"/>
+      <c r="L28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29">
+        <v>17</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>764</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="K29" s="7"/>
+      <c r="L29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30">
+        <v>18</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>522</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="K30" s="7"/>
+      <c r="L30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31">
+        <v>19</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>474</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="K31" s="9"/>
+      <c r="L31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32">
+        <v>20</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32">
+        <v>630</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="K32" s="9"/>
+      <c r="L32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33">
+        <v>21</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33">
+        <v>527</v>
+      </c>
+      <c r="F33">
+        <v>2</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="K33" s="9"/>
+      <c r="L33" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A34" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34">
+        <v>22</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>517</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="K34" s="7"/>
+      <c r="L34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35">
+        <v>23</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>527</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="K35" s="7"/>
+      <c r="L35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36">
+        <v>24</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>667</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <v>1</v>
+      </c>
+      <c r="K36" s="7"/>
+      <c r="L36" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37">
+        <v>25</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="E37">
+        <v>764</v>
+      </c>
+      <c r="F37">
+        <v>2</v>
+      </c>
+      <c r="I37">
+        <v>1</v>
+      </c>
+      <c r="K37" s="7"/>
+      <c r="L37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38">
+        <v>26</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+      <c r="E38">
+        <v>522</v>
+      </c>
+      <c r="F38">
+        <v>2</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="K38" s="7"/>
+      <c r="L38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>27</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>474</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="I39">
+        <v>1</v>
+      </c>
+      <c r="K39" s="9"/>
+      <c r="L39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>28</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>630</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
+      </c>
+      <c r="K40" s="9"/>
+      <c r="L40" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A41" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41">
+        <v>29</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>527</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <v>1</v>
+      </c>
+      <c r="K41" s="9"/>
+      <c r="L41" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A42" t="s">
+        <v>38</v>
+      </c>
+      <c r="B42">
+        <v>30</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42">
+        <v>517</v>
+      </c>
+      <c r="F42">
+        <v>2</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="K42" s="7"/>
+      <c r="L42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A43" t="s">
+        <v>38</v>
+      </c>
+      <c r="B43">
+        <v>31</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+      <c r="E43">
+        <v>527</v>
+      </c>
+      <c r="F43">
+        <v>2</v>
+      </c>
+      <c r="I43">
+        <v>1</v>
+      </c>
+      <c r="K43" s="7"/>
+      <c r="L43" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A44" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44">
+        <v>32</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>667</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+      <c r="K44" s="7"/>
+      <c r="L44" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A45" t="s">
+        <v>38</v>
+      </c>
+      <c r="B45">
+        <v>33</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>764</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="I45">
+        <v>1</v>
+      </c>
+      <c r="K45" s="7"/>
+      <c r="L45" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A46" t="s">
+        <v>38</v>
+      </c>
+      <c r="B46">
+        <v>34</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>522</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="I46">
+        <v>1</v>
+      </c>
+      <c r="K46" s="7"/>
+      <c r="L46" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A47" t="s">
+        <v>38</v>
+      </c>
+      <c r="B47">
+        <v>35</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="E47">
+        <v>474</v>
+      </c>
+      <c r="F47">
+        <v>2</v>
+      </c>
+      <c r="I47">
+        <v>1</v>
+      </c>
+      <c r="K47" s="9"/>
+      <c r="L47" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A48" t="s">
+        <v>38</v>
+      </c>
+      <c r="B48">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" ht="15.75" customHeight="1">
-      <c r="J13" s="7"/>
-    </row>
-    <row r="14" spans="1:16" ht="15.75" customHeight="1">
-      <c r="J14" s="7"/>
-    </row>
-    <row r="15" spans="1:16" ht="15.75" customHeight="1">
-      <c r="J15" s="9"/>
-    </row>
-    <row r="16" spans="1:16" ht="15.75" customHeight="1">
-      <c r="J16" s="9"/>
-    </row>
-    <row r="17" spans="10:10" ht="15.75" customHeight="1">
-      <c r="J17" s="9"/>
-    </row>
-    <row r="18" spans="10:10" ht="15.75" customHeight="1">
-      <c r="J18" s="7"/>
-    </row>
-    <row r="19" spans="10:10" ht="15.75" customHeight="1">
-      <c r="J19" s="7"/>
-    </row>
-    <row r="20" spans="10:10" ht="15.75" customHeight="1">
-      <c r="J20" s="7"/>
-    </row>
-    <row r="21" spans="10:10" ht="15.75" customHeight="1">
-      <c r="J21" s="7"/>
-    </row>
-    <row r="22" spans="10:10" ht="15.75" customHeight="1">
-      <c r="J22" s="7"/>
-    </row>
-    <row r="23" spans="10:10" ht="15.75" customHeight="1">
-      <c r="J23" s="9"/>
-    </row>
-    <row r="24" spans="10:10" ht="15.75" customHeight="1">
-      <c r="J24" s="9"/>
-    </row>
-    <row r="25" spans="10:10" ht="15.75" customHeight="1">
-      <c r="J25" s="9"/>
-    </row>
-    <row r="26" spans="10:10" ht="15.75" customHeight="1">
-      <c r="J26" s="7"/>
-    </row>
-    <row r="27" spans="10:10" ht="15.75" customHeight="1">
-      <c r="J27" s="7"/>
-    </row>
-    <row r="28" spans="10:10" ht="15.75" customHeight="1">
-      <c r="J28" s="7"/>
-    </row>
-    <row r="29" spans="10:10" ht="15.75" customHeight="1">
-      <c r="J29" s="7"/>
-    </row>
-    <row r="30" spans="10:10" ht="15.75" customHeight="1">
-      <c r="J30" s="7"/>
-    </row>
-    <row r="31" spans="10:10" ht="15.75" customHeight="1">
-      <c r="J31" s="9"/>
-    </row>
-    <row r="32" spans="10:10" ht="15.75" customHeight="1">
-      <c r="J32" s="9"/>
-    </row>
-    <row r="33" spans="10:10" ht="15.75" customHeight="1">
-      <c r="J33" s="9"/>
-    </row>
-    <row r="34" spans="10:10" ht="15.75" customHeight="1">
-      <c r="J34" s="7"/>
-    </row>
-    <row r="35" spans="10:10" ht="15.75" customHeight="1">
-      <c r="J35" s="7"/>
-    </row>
-    <row r="36" spans="10:10" ht="15.75" customHeight="1">
-      <c r="J36" s="7"/>
-    </row>
-    <row r="37" spans="10:10" ht="15.75" customHeight="1">
-      <c r="J37" s="7"/>
-    </row>
-    <row r="38" spans="10:10" ht="15.75" customHeight="1">
-      <c r="J38" s="7"/>
-    </row>
-    <row r="39" spans="10:10" ht="15.75" customHeight="1">
-      <c r="J39" s="9"/>
-    </row>
-    <row r="40" spans="10:10" ht="15.75" customHeight="1">
-      <c r="J40" s="9"/>
-    </row>
-    <row r="41" spans="10:10" ht="15.75" customHeight="1">
-      <c r="J41" s="9"/>
-    </row>
-    <row r="42" spans="10:10" ht="15.75" customHeight="1">
-      <c r="J42" s="7"/>
-    </row>
-    <row r="43" spans="10:10" ht="15.75" customHeight="1">
-      <c r="J43" s="7"/>
-    </row>
-    <row r="44" spans="10:10" ht="15.75" customHeight="1">
-      <c r="J44" s="7"/>
-    </row>
-    <row r="45" spans="10:10" ht="15.75" customHeight="1">
-      <c r="J45" s="7"/>
-    </row>
-    <row r="46" spans="10:10" ht="15.75" customHeight="1">
-      <c r="J46" s="7"/>
-    </row>
-    <row r="47" spans="10:10" ht="15.75" customHeight="1">
-      <c r="J47" s="9"/>
-    </row>
-    <row r="48" spans="10:10" ht="15.75" customHeight="1">
-      <c r="J48" s="7"/>
-    </row>
-    <row r="49" ht="15.75" customHeight="1"/>
-    <row r="50" ht="15.75" customHeight="1"/>
-    <row r="51" ht="15.75" customHeight="1"/>
-    <row r="52" ht="15.75" customHeight="1"/>
-    <row r="53" ht="15.75" customHeight="1"/>
-    <row r="54" ht="15.75" customHeight="1"/>
-    <row r="55" ht="15.75" customHeight="1"/>
-    <row r="56" ht="15.75" customHeight="1"/>
-    <row r="57" ht="15.75" customHeight="1"/>
-    <row r="58" ht="15.75" customHeight="1"/>
-    <row r="59" ht="15.75" customHeight="1"/>
-    <row r="60" ht="15.75" customHeight="1"/>
-    <row r="61" ht="15.75" customHeight="1"/>
-    <row r="62" ht="15.75" customHeight="1"/>
-    <row r="63" ht="15.75" customHeight="1"/>
-    <row r="64" ht="15.75" customHeight="1"/>
-    <row r="65" ht="15.75" customHeight="1"/>
-    <row r="66" ht="15.75" customHeight="1"/>
-    <row r="67" ht="15.75" customHeight="1"/>
-    <row r="68" ht="15.75" customHeight="1"/>
-    <row r="69" ht="15.75" customHeight="1"/>
-    <row r="70" ht="15.75" customHeight="1"/>
-    <row r="71" ht="15.75" customHeight="1"/>
-    <row r="72" ht="15.75" customHeight="1"/>
-    <row r="73" ht="15.75" customHeight="1"/>
-    <row r="74" ht="15.75" customHeight="1"/>
-    <row r="75" ht="15.75" customHeight="1"/>
-    <row r="76" ht="15.75" customHeight="1"/>
-    <row r="77" ht="15.75" customHeight="1"/>
-    <row r="78" ht="15.75" customHeight="1"/>
-    <row r="79" ht="15.75" customHeight="1"/>
-    <row r="80" ht="15.75" customHeight="1"/>
-    <row r="81" ht="15.75" customHeight="1"/>
-    <row r="82" ht="15.75" customHeight="1"/>
-    <row r="83" ht="15.75" customHeight="1"/>
-    <row r="84" ht="15.75" customHeight="1"/>
-    <row r="85" ht="15.75" customHeight="1"/>
-    <row r="86" ht="15.75" customHeight="1"/>
-    <row r="87" ht="15.75" customHeight="1"/>
-    <row r="88" ht="15.75" customHeight="1"/>
-    <row r="89" ht="15.75" customHeight="1"/>
-    <row r="90" ht="15.75" customHeight="1"/>
-    <row r="91" ht="15.75" customHeight="1"/>
-    <row r="92" ht="15.75" customHeight="1"/>
-    <row r="93" ht="15.75" customHeight="1"/>
-    <row r="94" ht="15.75" customHeight="1"/>
-    <row r="95" ht="15.75" customHeight="1"/>
-    <row r="96" ht="15.75" customHeight="1"/>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="E48">
+        <v>554</v>
+      </c>
+      <c r="F48">
+        <v>2</v>
+      </c>
+      <c r="I48">
+        <v>1</v>
+      </c>
+      <c r="K48" s="7"/>
+      <c r="L48" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A49" t="s">
+        <v>38</v>
+      </c>
+      <c r="B49">
+        <v>37</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>802</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="I49">
+        <v>1</v>
+      </c>
+      <c r="L49" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A50" t="s">
+        <v>38</v>
+      </c>
+      <c r="B50">
+        <v>38</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>802</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="I50">
+        <v>1</v>
+      </c>
+      <c r="L50" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A51" t="s">
+        <v>38</v>
+      </c>
+      <c r="B51">
+        <v>39</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>727</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+      <c r="L51" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A52" t="s">
+        <v>38</v>
+      </c>
+      <c r="B52">
+        <v>40</v>
+      </c>
+      <c r="C52">
+        <v>2</v>
+      </c>
+      <c r="D52">
+        <v>2</v>
+      </c>
+      <c r="E52">
+        <v>764</v>
+      </c>
+      <c r="F52">
+        <v>2</v>
+      </c>
+      <c r="I52">
+        <v>1</v>
+      </c>
+      <c r="L52" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A53" t="s">
+        <v>38</v>
+      </c>
+      <c r="B53">
+        <v>41</v>
+      </c>
+      <c r="C53">
+        <v>2</v>
+      </c>
+      <c r="D53">
+        <v>2</v>
+      </c>
+      <c r="E53">
+        <v>522</v>
+      </c>
+      <c r="F53">
+        <v>2</v>
+      </c>
+      <c r="I53">
+        <v>1</v>
+      </c>
+      <c r="L53" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A54" t="s">
+        <v>38</v>
+      </c>
+      <c r="B54">
+        <v>42</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>474</v>
+      </c>
+      <c r="F54">
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
+      <c r="L54" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A55" t="s">
+        <v>38</v>
+      </c>
+      <c r="B55">
+        <v>43</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>680</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="I55">
+        <v>1</v>
+      </c>
+      <c r="L55" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A56" t="s">
+        <v>38</v>
+      </c>
+      <c r="B56">
+        <v>44</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>802</v>
+      </c>
+      <c r="F56">
+        <v>1</v>
+      </c>
+      <c r="I56">
+        <v>1</v>
+      </c>
+      <c r="L56" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A57" t="s">
+        <v>38</v>
+      </c>
+      <c r="B57">
+        <v>45</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="E57">
+        <v>802</v>
+      </c>
+      <c r="F57">
+        <v>2</v>
+      </c>
+      <c r="I57">
+        <v>1</v>
+      </c>
+      <c r="L57" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A58" t="s">
+        <v>38</v>
+      </c>
+      <c r="B58">
+        <v>46</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>2</v>
+      </c>
+      <c r="E58">
+        <v>727</v>
+      </c>
+      <c r="F58">
+        <v>2</v>
+      </c>
+      <c r="I58">
+        <v>1</v>
+      </c>
+      <c r="L58" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A59" t="s">
+        <v>38</v>
+      </c>
+      <c r="B59">
+        <v>47</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>764</v>
+      </c>
+      <c r="F59">
+        <v>1</v>
+      </c>
+      <c r="I59">
+        <v>1</v>
+      </c>
+      <c r="L59" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A60" t="s">
+        <v>38</v>
+      </c>
+      <c r="B60">
+        <v>48</v>
+      </c>
+      <c r="C60">
+        <v>2</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>522</v>
+      </c>
+      <c r="F60">
+        <v>1</v>
+      </c>
+      <c r="I60">
+        <v>1</v>
+      </c>
+      <c r="L60" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A61" t="s">
+        <v>38</v>
+      </c>
+      <c r="B61">
+        <v>49</v>
+      </c>
+      <c r="C61">
+        <v>2</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>474</v>
+      </c>
+      <c r="F61">
+        <v>1</v>
+      </c>
+      <c r="I61">
+        <v>1</v>
+      </c>
+      <c r="L61" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A62" t="s">
+        <v>38</v>
+      </c>
+      <c r="B62">
+        <v>50</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>2</v>
+      </c>
+      <c r="E62">
+        <v>680</v>
+      </c>
+      <c r="F62">
+        <v>2</v>
+      </c>
+      <c r="I62">
+        <v>1</v>
+      </c>
+      <c r="L62" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A63" t="s">
+        <v>38</v>
+      </c>
+      <c r="B63">
+        <v>51</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63">
+        <v>2</v>
+      </c>
+      <c r="E63">
+        <v>802</v>
+      </c>
+      <c r="F63">
+        <v>2</v>
+      </c>
+      <c r="I63">
+        <v>1</v>
+      </c>
+      <c r="L63" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A64" t="s">
+        <v>38</v>
+      </c>
+      <c r="B64">
+        <v>52</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>802</v>
+      </c>
+      <c r="F64">
+        <v>1</v>
+      </c>
+      <c r="I64">
+        <v>1</v>
+      </c>
+      <c r="L64" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A65" t="s">
+        <v>38</v>
+      </c>
+      <c r="B65">
+        <v>53</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <v>727</v>
+      </c>
+      <c r="F65">
+        <v>1</v>
+      </c>
+      <c r="I65">
+        <v>1</v>
+      </c>
+      <c r="L65" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A66" t="s">
+        <v>38</v>
+      </c>
+      <c r="B66">
+        <v>54</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>775</v>
+      </c>
+      <c r="F66">
+        <v>1</v>
+      </c>
+      <c r="I66">
+        <v>1</v>
+      </c>
+      <c r="L66" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A67" t="s">
+        <v>38</v>
+      </c>
+      <c r="B67">
+        <v>55</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+      <c r="D67">
+        <v>2</v>
+      </c>
+      <c r="E67">
+        <v>522</v>
+      </c>
+      <c r="F67">
+        <v>2</v>
+      </c>
+      <c r="I67">
+        <v>1</v>
+      </c>
+      <c r="L67" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A68" t="s">
+        <v>38</v>
+      </c>
+      <c r="B68">
+        <v>56</v>
+      </c>
+      <c r="C68">
+        <v>2</v>
+      </c>
+      <c r="D68">
+        <v>2</v>
+      </c>
+      <c r="E68">
+        <v>474</v>
+      </c>
+      <c r="F68">
+        <v>2</v>
+      </c>
+      <c r="I68">
+        <v>1</v>
+      </c>
+      <c r="L68" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A69" t="s">
+        <v>38</v>
+      </c>
+      <c r="B69">
+        <v>57</v>
+      </c>
+      <c r="C69">
+        <v>2</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69">
+        <v>680</v>
+      </c>
+      <c r="F69">
+        <v>1</v>
+      </c>
+      <c r="I69">
+        <v>1</v>
+      </c>
+      <c r="L69" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A70" t="s">
+        <v>38</v>
+      </c>
+      <c r="B70">
+        <v>58</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70">
+        <v>802</v>
+      </c>
+      <c r="F70">
+        <v>1</v>
+      </c>
+      <c r="I70">
+        <v>1</v>
+      </c>
+      <c r="L70" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A71" t="s">
+        <v>38</v>
+      </c>
+      <c r="B71">
+        <v>59</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71">
+        <v>802</v>
+      </c>
+      <c r="F71">
+        <v>1</v>
+      </c>
+      <c r="I71">
+        <v>1</v>
+      </c>
+      <c r="L71" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A72" t="s">
+        <v>38</v>
+      </c>
+      <c r="B72">
+        <v>60</v>
+      </c>
+      <c r="C72">
+        <v>1</v>
+      </c>
+      <c r="D72">
+        <v>2</v>
+      </c>
+      <c r="E72">
+        <v>727</v>
+      </c>
+      <c r="F72">
+        <v>2</v>
+      </c>
+      <c r="I72">
+        <v>1</v>
+      </c>
+      <c r="L72" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A73" t="s">
+        <v>38</v>
+      </c>
+      <c r="B73">
+        <v>61</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="E73">
+        <v>775</v>
+      </c>
+      <c r="F73">
+        <v>1</v>
+      </c>
+      <c r="I73">
+        <v>1</v>
+      </c>
+      <c r="L73" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A74" t="s">
+        <v>38</v>
+      </c>
+      <c r="B74">
+        <v>62</v>
+      </c>
+      <c r="C74">
+        <v>1</v>
+      </c>
+      <c r="D74">
+        <v>2</v>
+      </c>
+      <c r="E74">
+        <v>522</v>
+      </c>
+      <c r="F74">
+        <v>1</v>
+      </c>
+      <c r="I74">
+        <v>1</v>
+      </c>
+      <c r="L74" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A75" t="s">
+        <v>38</v>
+      </c>
+      <c r="B75">
+        <v>63</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="D75">
+        <v>2</v>
+      </c>
+      <c r="E75">
+        <v>474</v>
+      </c>
+      <c r="F75">
+        <v>1</v>
+      </c>
+      <c r="I75">
+        <v>1</v>
+      </c>
+      <c r="L75" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A76" t="s">
+        <v>38</v>
+      </c>
+      <c r="B76">
+        <v>64</v>
+      </c>
+      <c r="C76">
+        <v>2</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
+      <c r="E76">
+        <v>680</v>
+      </c>
+      <c r="F76">
+        <v>2</v>
+      </c>
+      <c r="I76">
+        <v>1</v>
+      </c>
+      <c r="L76" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A77" t="s">
+        <v>38</v>
+      </c>
+      <c r="B77">
+        <v>65</v>
+      </c>
+      <c r="C77">
+        <v>9</v>
+      </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
+      <c r="E77">
+        <v>802</v>
+      </c>
+      <c r="F77">
+        <v>2</v>
+      </c>
+      <c r="I77">
+        <v>1</v>
+      </c>
+      <c r="L77" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A78" t="s">
+        <v>38</v>
+      </c>
+      <c r="B78">
+        <v>66</v>
+      </c>
+      <c r="C78">
+        <v>9</v>
+      </c>
+      <c r="D78">
+        <v>2</v>
+      </c>
+      <c r="E78">
+        <v>802</v>
+      </c>
+      <c r="F78">
+        <v>1</v>
+      </c>
+      <c r="I78">
+        <v>1</v>
+      </c>
+      <c r="L78" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A79" t="s">
+        <v>38</v>
+      </c>
+      <c r="B79">
+        <v>67</v>
+      </c>
+      <c r="C79">
+        <v>9</v>
+      </c>
+      <c r="D79">
+        <v>2</v>
+      </c>
+      <c r="E79">
+        <v>727</v>
+      </c>
+      <c r="F79">
+        <v>1</v>
+      </c>
+      <c r="I79">
+        <v>1</v>
+      </c>
+      <c r="L79" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A80" t="s">
+        <v>38</v>
+      </c>
+      <c r="B80">
+        <v>68</v>
+      </c>
+      <c r="C80">
+        <v>10</v>
+      </c>
+      <c r="D80">
+        <v>3</v>
+      </c>
+      <c r="E80">
+        <v>1082</v>
+      </c>
+      <c r="F80">
+        <v>1</v>
+      </c>
+      <c r="I80">
+        <v>1</v>
+      </c>
+      <c r="L80" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A81" t="s">
+        <v>38</v>
+      </c>
+      <c r="B81">
+        <v>69</v>
+      </c>
+      <c r="C81">
+        <v>10</v>
+      </c>
+      <c r="D81">
+        <v>3</v>
+      </c>
+      <c r="E81">
+        <v>1044</v>
+      </c>
+      <c r="F81">
+        <v>2</v>
+      </c>
+      <c r="I81">
+        <v>1</v>
+      </c>
+      <c r="L81" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A82" t="s">
+        <v>38</v>
+      </c>
+      <c r="B82">
+        <v>70</v>
+      </c>
+      <c r="C82">
+        <v>11</v>
+      </c>
+      <c r="D82">
+        <v>2</v>
+      </c>
+      <c r="E82">
+        <v>770</v>
+      </c>
+      <c r="F82">
+        <v>2</v>
+      </c>
+      <c r="I82">
+        <v>1</v>
+      </c>
+      <c r="L82" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A83" t="s">
+        <v>38</v>
+      </c>
+      <c r="B83">
+        <v>71</v>
+      </c>
+      <c r="C83">
+        <v>11</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+      <c r="E83">
+        <v>522</v>
+      </c>
+      <c r="F83">
+        <v>1</v>
+      </c>
+      <c r="I83">
+        <v>0</v>
+      </c>
+      <c r="L83" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A84" t="s">
+        <v>38</v>
+      </c>
+      <c r="B84">
+        <v>72</v>
+      </c>
+      <c r="C84">
+        <v>11</v>
+      </c>
+      <c r="D84">
+        <v>2</v>
+      </c>
+      <c r="E84">
+        <v>802</v>
+      </c>
+      <c r="F84">
+        <v>1</v>
+      </c>
+      <c r="I84">
+        <v>1</v>
+      </c>
+      <c r="L84" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A85" t="s">
+        <v>38</v>
+      </c>
+      <c r="B85">
+        <v>73</v>
+      </c>
+      <c r="C85">
+        <v>12</v>
+      </c>
+      <c r="D85">
+        <v>2</v>
+      </c>
+      <c r="E85">
+        <v>770</v>
+      </c>
+      <c r="F85">
+        <v>1</v>
+      </c>
+      <c r="I85">
+        <v>1</v>
+      </c>
+      <c r="L85" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A86" t="s">
+        <v>38</v>
+      </c>
+      <c r="B86">
+        <v>74</v>
+      </c>
+      <c r="C86">
+        <v>12</v>
+      </c>
+      <c r="D86">
+        <v>1</v>
+      </c>
+      <c r="E86">
+        <v>522</v>
+      </c>
+      <c r="F86">
+        <v>2</v>
+      </c>
+      <c r="I86">
+        <v>0</v>
+      </c>
+      <c r="L86" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A87" t="s">
+        <v>38</v>
+      </c>
+      <c r="B87">
+        <v>75</v>
+      </c>
+      <c r="C87">
+        <v>12</v>
+      </c>
+      <c r="D87">
+        <v>2</v>
+      </c>
+      <c r="E87">
+        <v>802</v>
+      </c>
+      <c r="F87">
+        <v>2</v>
+      </c>
+      <c r="I87">
+        <v>1</v>
+      </c>
+      <c r="L87" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" ht="15.75" customHeight="1"/>
+    <row r="89" spans="1:12" ht="15.75" customHeight="1"/>
+    <row r="90" spans="1:12" ht="15.75" customHeight="1"/>
+    <row r="91" spans="1:12" ht="15.75" customHeight="1"/>
+    <row r="92" spans="1:12" ht="15.75" customHeight="1"/>
+    <row r="93" spans="1:12" ht="15.75" customHeight="1"/>
+    <row r="94" spans="1:12" ht="15.75" customHeight="1"/>
+    <row r="95" spans="1:12" ht="15.75" customHeight="1"/>
+    <row r="96" spans="1:12" ht="15.75" customHeight="1"/>
     <row r="97" ht="15.75" customHeight="1"/>
     <row r="98" ht="15.75" customHeight="1"/>
     <row r="99" ht="15.75" customHeight="1"/>
@@ -1886,7 +3790,7 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
   </sheetData>
-  <autoFilter ref="A1:W999" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:X999" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>

</xml_diff>